<commit_message>
base de datos con password
</commit_message>
<xml_diff>
--- a/db/datosTablas.xlsx
+++ b/db/datosTablas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uriel\Documents\GitHub\Proyecto_PA_2020\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84CB80B9-9487-4E77-8E9C-AEB44AC7200A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B94C7B-8745-4EE7-A34A-635A0F681611}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3BA2B90A-A5E0-48C3-A110-4AABBF910E3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{3BA2B90A-A5E0-48C3-A110-4AABBF910E3D}"/>
   </bookViews>
   <sheets>
     <sheet name="salones" sheetId="12" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="245">
   <si>
     <t>id_salon</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>id_numCuentaProf</t>
-  </si>
-  <si>
-    <t>id_nivel1</t>
   </si>
   <si>
     <t>nombreProf</t>
@@ -762,6 +759,72 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>password_1</t>
+  </si>
+  <si>
+    <t>password_2</t>
+  </si>
+  <si>
+    <t>password_3</t>
+  </si>
+  <si>
+    <t>password_4</t>
+  </si>
+  <si>
+    <t>password_0</t>
+  </si>
+  <si>
+    <t>password_5</t>
+  </si>
+  <si>
+    <t>password_6</t>
+  </si>
+  <si>
+    <t>password_7</t>
+  </si>
+  <si>
+    <t>password_8</t>
+  </si>
+  <si>
+    <t>password_9</t>
+  </si>
+  <si>
+    <t>password_10</t>
+  </si>
+  <si>
+    <t>password_11</t>
+  </si>
+  <si>
+    <t>password_12</t>
+  </si>
+  <si>
+    <t>password_13</t>
+  </si>
+  <si>
+    <t>password_14</t>
+  </si>
+  <si>
+    <t>password_15</t>
+  </si>
+  <si>
+    <t>password_16</t>
+  </si>
+  <si>
+    <t>password_17</t>
+  </si>
+  <si>
+    <t>password_18</t>
+  </si>
+  <si>
+    <t>password_19</t>
+  </si>
+  <si>
+    <t>passwordProf</t>
   </si>
 </sst>
 </file>
@@ -771,7 +834,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,6 +854,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1144,7 +1213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34AFB3E8-1FA2-40B0-9A29-B6E0C2ED18CB}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10:D12"/>
     </sheetView>
   </sheetViews>
@@ -1281,7 +1350,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C10">
         <v>25</v>
@@ -1295,7 +1364,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -1309,7 +1378,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C12">
         <v>25</v>
@@ -1641,10 +1710,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
         <v>119</v>
-      </c>
-      <c r="B1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1688,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96CD15D-F95E-4208-8C31-8C3F1885D763}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1705,54 +1774,54 @@
         <v>59</v>
       </c>
       <c r="B1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
         <v>89</v>
       </c>
-      <c r="G1" t="s">
-        <v>90</v>
-      </c>
       <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>104</v>
-      </c>
-      <c r="J1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>228</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
         <v>86</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
       </c>
       <c r="F2" s="4">
         <v>32642</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H2">
         <v>56345</v>
@@ -1761,30 +1830,30 @@
         <v>5525659589</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F3" s="4">
         <v>32994</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3">
         <v>57895</v>
@@ -1793,30 +1862,30 @@
         <v>5583854514</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>225</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" s="4">
         <v>25684</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H4">
         <v>59445</v>
@@ -1825,30 +1894,30 @@
         <v>5642049439</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>226</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F5" s="4">
         <v>31368</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H5">
         <v>60995</v>
@@ -1857,30 +1926,30 @@
         <v>5700244364</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>227</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F6" s="4">
         <v>32424</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H6">
         <v>62545</v>
@@ -1889,30 +1958,30 @@
         <v>5758439289</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>229</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="4">
         <v>29554</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H7">
         <v>64095</v>
@@ -1921,30 +1990,30 @@
         <v>5816634214</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>230</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F8" s="4">
         <v>24999</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H8">
         <v>65645</v>
@@ -1953,30 +2022,30 @@
         <v>5874829139</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>231</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" s="4">
         <v>34049</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H9">
         <v>67195</v>
@@ -1985,30 +2054,30 @@
         <v>5933024064</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>232</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F10" s="4">
         <v>27432</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H10">
         <v>68745</v>
@@ -2017,30 +2086,30 @@
         <v>5991218989</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>233</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" s="4">
         <v>21775</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H11">
         <v>70295</v>
@@ -2049,30 +2118,30 @@
         <v>6049413914</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>234</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F12" s="4">
         <v>31536</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H12">
         <v>71845</v>
@@ -2081,30 +2150,30 @@
         <v>6107608839</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
+        <v>111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>235</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F13" s="4">
         <v>33618</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H13">
         <v>73395</v>
@@ -2113,10 +2182,11 @@
         <v>6165803764</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{BC915649-7FA9-41EC-B418-1FE78B73B241}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{459D0318-45B4-4836-852C-8928FF2CD0EB}"/>
@@ -2137,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4418968-788A-443B-A486-D91705524332}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2149,50 +2219,54 @@
     <col min="3" max="3" width="17.77734375" customWidth="1"/>
     <col min="6" max="6" width="15.44140625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="11" max="11" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
         <v>121</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" t="s">
         <v>122</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>123</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>124</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>125</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>126</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>127</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>130</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>131</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>132</v>
       </c>
-      <c r="M1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -2200,40 +2274,43 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>228</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="6">
+        <v>149</v>
+      </c>
+      <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="6">
         <v>39582</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="H2">
+      <c r="H2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2">
         <v>86842</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>5524568989</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="K2">
+      <c r="K2" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="L2">
         <v>0</v>
       </c>
-      <c r="L2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M2">
+      <c r="M2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N2">
         <v>2008</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -2241,40 +2318,43 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>224</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="6">
+        <v>150</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="6">
         <v>39612</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H3">
+      <c r="H3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3">
         <v>55565</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5524868982</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="K3">
+      <c r="K3" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="L3">
         <v>0</v>
       </c>
-      <c r="L3" t="s">
-        <v>167</v>
-      </c>
-      <c r="M3">
+      <c r="M3" t="s">
+        <v>166</v>
+      </c>
+      <c r="N3">
         <v>2008</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1002</v>
       </c>
@@ -2282,40 +2362,43 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>225</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="6">
+        <v>151</v>
+      </c>
+      <c r="F4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="6">
         <v>39642</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H4">
+      <c r="H4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I4">
         <v>58954</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>5525168975</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="K4">
+      <c r="K4" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="L4">
         <v>0</v>
       </c>
-      <c r="L4" t="s">
-        <v>167</v>
-      </c>
-      <c r="M4">
+      <c r="M4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N4">
         <v>2008</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -2323,40 +2406,43 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>226</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" s="6">
+        <v>152</v>
+      </c>
+      <c r="F5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="6">
         <v>39672</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="H5">
+      <c r="H5" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I5">
         <v>57577</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>5525468968</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="K5">
+      <c r="K5" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="L5">
         <v>0</v>
       </c>
-      <c r="L5" t="s">
-        <v>167</v>
-      </c>
-      <c r="M5">
+      <c r="M5" t="s">
+        <v>166</v>
+      </c>
+      <c r="N5">
         <v>2008</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1004</v>
       </c>
@@ -2364,40 +2450,43 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>227</v>
       </c>
       <c r="D6" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="6">
+        <v>153</v>
+      </c>
+      <c r="F6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="6">
         <v>39702</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H6">
+      <c r="H6" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I6">
         <v>54757</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>5525768961</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="K6">
+      <c r="K6" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="L6" t="s">
-        <v>167</v>
-      </c>
-      <c r="M6">
+      <c r="M6" t="s">
+        <v>166</v>
+      </c>
+      <c r="N6">
         <v>2008</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1005</v>
       </c>
@@ -2405,40 +2494,43 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="6">
+        <v>154</v>
+      </c>
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="6">
         <v>39216</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="H7">
+      <c r="H7" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I7">
         <v>45578</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>5526068954</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="K7">
+      <c r="K7" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="L7">
         <v>9.4</v>
       </c>
-      <c r="L7" t="s">
-        <v>167</v>
-      </c>
-      <c r="M7">
+      <c r="M7" t="s">
+        <v>166</v>
+      </c>
+      <c r="N7">
         <v>2007</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1006</v>
       </c>
@@ -2446,40 +2538,43 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>230</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="6">
+        <v>155</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="6">
         <v>39246</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="H8">
+      <c r="H8" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="I8">
         <v>57857</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>5526368947</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="K8">
+      <c r="K8" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="L8">
         <v>8.6</v>
       </c>
-      <c r="L8" t="s">
-        <v>167</v>
-      </c>
-      <c r="M8">
+      <c r="M8" t="s">
+        <v>166</v>
+      </c>
+      <c r="N8">
         <v>2007</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1007</v>
       </c>
@@ -2487,40 +2582,43 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>231</v>
       </c>
       <c r="D9" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" s="6">
+        <v>198</v>
+      </c>
+      <c r="F9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="6">
         <v>39276</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="H9">
+      <c r="H9" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="I9">
         <v>45455</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>5526668940</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="K9">
+      <c r="K9" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="L9">
         <v>7.8</v>
       </c>
-      <c r="L9" t="s">
-        <v>168</v>
-      </c>
-      <c r="M9">
+      <c r="M9" t="s">
+        <v>167</v>
+      </c>
+      <c r="N9">
         <v>2007</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1008</v>
       </c>
@@ -2528,40 +2626,43 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" t="s">
         <v>169</v>
       </c>
-      <c r="D10" t="s">
-        <v>170</v>
-      </c>
-      <c r="E10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="F10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="6">
         <v>39306</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="H10">
+      <c r="H10" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10">
         <v>49507</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>5526968933</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="K10">
+      <c r="K10" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="L10">
         <v>7</v>
       </c>
-      <c r="L10" t="s">
-        <v>167</v>
-      </c>
-      <c r="M10">
+      <c r="M10" t="s">
+        <v>166</v>
+      </c>
+      <c r="N10">
         <v>2007</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1009</v>
       </c>
@@ -2569,40 +2670,43 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>233</v>
       </c>
       <c r="D11" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="6">
+        <v>156</v>
+      </c>
+      <c r="F11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="6">
         <v>39336</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="H11">
+      <c r="H11" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I11">
         <v>49445</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>5527268926</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="K11">
+      <c r="K11" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="L11">
         <v>6.2</v>
       </c>
-      <c r="L11" t="s">
-        <v>167</v>
-      </c>
-      <c r="M11">
+      <c r="M11" t="s">
+        <v>166</v>
+      </c>
+      <c r="N11">
         <v>2007</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1010</v>
       </c>
@@ -2610,40 +2714,43 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>234</v>
       </c>
       <c r="D12" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" s="6">
+        <v>157</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="6">
         <v>38851</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="H12">
+      <c r="H12" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I12">
         <v>49384</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>5527568919</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="K12">
+      <c r="K12" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="L12">
         <v>9.4</v>
       </c>
-      <c r="L12" t="s">
-        <v>167</v>
-      </c>
-      <c r="M12">
+      <c r="M12" t="s">
+        <v>166</v>
+      </c>
+      <c r="N12">
         <v>2006</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1011</v>
       </c>
@@ -2651,40 +2758,43 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>235</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="6">
+        <v>158</v>
+      </c>
+      <c r="F13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="6">
         <v>38881</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H13">
+      <c r="H13" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13">
         <v>49322</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>5527868912</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="K13">
+      <c r="K13" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="L13">
         <v>8.6</v>
       </c>
-      <c r="L13" t="s">
-        <v>167</v>
-      </c>
-      <c r="M13">
+      <c r="M13" t="s">
+        <v>166</v>
+      </c>
+      <c r="N13">
         <v>2006</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1012</v>
       </c>
@@ -2692,40 +2802,43 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>236</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="6">
+        <v>159</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="6">
         <v>38911</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="H14">
+      <c r="H14" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I14">
         <v>49261</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>5528168905</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="K14">
+      <c r="K14" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="L14">
         <v>7.8</v>
       </c>
-      <c r="L14" t="s">
-        <v>167</v>
-      </c>
-      <c r="M14">
+      <c r="M14" t="s">
+        <v>166</v>
+      </c>
+      <c r="N14">
         <v>2006</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1013</v>
       </c>
@@ -2733,40 +2846,43 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
+        <v>237</v>
       </c>
       <c r="D15" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="6">
+        <v>160</v>
+      </c>
+      <c r="F15" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="6">
         <v>38941</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H15">
+      <c r="H15" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I15">
         <v>57575</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>5528468898</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="K15">
+      <c r="K15" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="L15">
         <v>7</v>
       </c>
-      <c r="L15" t="s">
-        <v>167</v>
-      </c>
-      <c r="M15">
+      <c r="M15" t="s">
+        <v>166</v>
+      </c>
+      <c r="N15">
         <v>2006</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1014</v>
       </c>
@@ -2774,40 +2890,43 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>238</v>
       </c>
       <c r="D16" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="6">
+        <v>157</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="6">
         <v>38971</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H16">
+      <c r="H16" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I16">
         <v>42757</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>5528768891</v>
       </c>
-      <c r="J16" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="K16">
+      <c r="K16" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="L16">
         <v>6.2</v>
       </c>
-      <c r="L16" t="s">
-        <v>167</v>
-      </c>
-      <c r="M16">
+      <c r="M16" t="s">
+        <v>166</v>
+      </c>
+      <c r="N16">
         <v>2006</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1015</v>
       </c>
@@ -2815,40 +2934,43 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>239</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="6">
+        <v>161</v>
+      </c>
+      <c r="F17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="6">
         <v>38486</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="H17">
+      <c r="H17" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I17">
         <v>77757</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>5529068884</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="K17">
+      <c r="K17" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="L17">
         <v>9.4</v>
       </c>
-      <c r="L17" t="s">
-        <v>167</v>
-      </c>
-      <c r="M17">
+      <c r="M17" t="s">
+        <v>166</v>
+      </c>
+      <c r="N17">
         <v>2005</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1016</v>
       </c>
@@ -2856,40 +2978,43 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
+        <v>240</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="6">
+        <v>162</v>
+      </c>
+      <c r="F18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="6">
         <v>38516</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H18">
+      <c r="H18" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I18">
         <v>75757</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>5529368877</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="K18">
+      <c r="K18" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="L18">
         <v>8.6</v>
       </c>
-      <c r="L18" t="s">
-        <v>167</v>
-      </c>
-      <c r="M18">
+      <c r="M18" t="s">
+        <v>166</v>
+      </c>
+      <c r="N18">
         <v>2005</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1017</v>
       </c>
@@ -2897,40 +3022,43 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>241</v>
       </c>
       <c r="D19" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="6">
+        <v>163</v>
+      </c>
+      <c r="F19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="6">
         <v>38546</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H19">
+      <c r="H19" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I19">
         <v>45757</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>5529668870</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="K19">
+      <c r="K19" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="L19">
         <v>7.8</v>
       </c>
-      <c r="L19" t="s">
-        <v>167</v>
-      </c>
-      <c r="M19">
+      <c r="M19" t="s">
+        <v>166</v>
+      </c>
+      <c r="N19">
         <v>2005</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1018</v>
       </c>
@@ -2938,40 +3066,43 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
+        <v>242</v>
+      </c>
+      <c r="D20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="6">
+        <v>38576</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I20">
+        <v>57577</v>
+      </c>
+      <c r="J20">
+        <v>5529968863</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="L20">
+        <v>7</v>
+      </c>
+      <c r="M20" t="s">
         <v>166</v>
       </c>
-      <c r="D20" t="s">
-        <v>161</v>
-      </c>
-      <c r="E20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="6">
-        <v>38576</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="H20">
-        <v>57577</v>
-      </c>
-      <c r="I20">
-        <v>5529968863</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="K20">
-        <v>7</v>
-      </c>
-      <c r="L20" t="s">
-        <v>167</v>
-      </c>
-      <c r="M20">
+      <c r="N20">
         <v>2005</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1019</v>
       </c>
@@ -2979,61 +3110,65 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>243</v>
       </c>
       <c r="D21" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="6">
+        <v>164</v>
+      </c>
+      <c r="F21" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="6">
         <v>38606</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H21">
+      <c r="H21" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I21">
         <v>57578</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>5530268856</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="K21">
+      <c r="K21" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="L21">
         <v>6.2</v>
       </c>
-      <c r="L21" t="s">
-        <v>167</v>
-      </c>
-      <c r="M21">
+      <c r="M21" t="s">
+        <v>166</v>
+      </c>
+      <c r="N21">
         <v>2005</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{BEB2FD88-6E18-4295-BC3E-054C0908ADCE}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{CB1A29C4-418C-4370-A340-D19868A9C208}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{2415E939-B57C-4FED-AE37-20B2BB7F5C63}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{A53648B5-383E-413A-BF3E-CDB2AD117299}"/>
-    <hyperlink ref="J6" r:id="rId5" xr:uid="{A03B98F7-DE36-43AB-83A6-47EB8792FA62}"/>
-    <hyperlink ref="J7" r:id="rId6" xr:uid="{9F53AAF3-B239-456A-8553-D6DD24A772D4}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{BB739991-1412-480D-AB0C-3DB8754E3628}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{61569326-95D6-42F5-B8A4-0501EB3CD3B2}"/>
-    <hyperlink ref="J10" r:id="rId9" xr:uid="{5399D83F-8F2D-4F9E-AE8A-18A9DEF63A48}"/>
-    <hyperlink ref="J11" r:id="rId10" xr:uid="{2DBA677F-388E-4417-A87B-EFEEF9330B11}"/>
-    <hyperlink ref="J12" r:id="rId11" xr:uid="{83E0E3A8-8DBB-41C2-A07D-E46E9F04E90B}"/>
-    <hyperlink ref="J13" r:id="rId12" xr:uid="{C75261D1-8074-4479-A01B-A7E7E9177687}"/>
-    <hyperlink ref="J14" r:id="rId13" xr:uid="{ABAB244F-6832-41C3-B584-145326DC26EA}"/>
-    <hyperlink ref="J15" r:id="rId14" xr:uid="{2D7A65A3-4A06-4F98-AD11-AFACE3C6198E}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{505E0218-2E89-44C5-8F7E-B4933A972984}"/>
-    <hyperlink ref="J17" r:id="rId16" xr:uid="{E74418DE-8B78-4447-9593-586192D39C59}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{487EFA46-35B6-4A6F-ADD1-8F9089FA752D}"/>
-    <hyperlink ref="J19" r:id="rId18" xr:uid="{9359AC1A-2F35-442F-BB5A-D7387CAFE419}"/>
-    <hyperlink ref="J20" r:id="rId19" xr:uid="{47476116-35F2-4366-8C0E-0E11F7C3F97D}"/>
-    <hyperlink ref="J21" r:id="rId20" xr:uid="{A3A33567-F1D4-45F5-BBB4-E3BC1DE171DD}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{BEB2FD88-6E18-4295-BC3E-054C0908ADCE}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{CB1A29C4-418C-4370-A340-D19868A9C208}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{2415E939-B57C-4FED-AE37-20B2BB7F5C63}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{A53648B5-383E-413A-BF3E-CDB2AD117299}"/>
+    <hyperlink ref="K6" r:id="rId5" xr:uid="{A03B98F7-DE36-43AB-83A6-47EB8792FA62}"/>
+    <hyperlink ref="K7" r:id="rId6" xr:uid="{9F53AAF3-B239-456A-8553-D6DD24A772D4}"/>
+    <hyperlink ref="K8" r:id="rId7" xr:uid="{BB739991-1412-480D-AB0C-3DB8754E3628}"/>
+    <hyperlink ref="K9" r:id="rId8" xr:uid="{61569326-95D6-42F5-B8A4-0501EB3CD3B2}"/>
+    <hyperlink ref="K10" r:id="rId9" xr:uid="{5399D83F-8F2D-4F9E-AE8A-18A9DEF63A48}"/>
+    <hyperlink ref="K11" r:id="rId10" xr:uid="{2DBA677F-388E-4417-A87B-EFEEF9330B11}"/>
+    <hyperlink ref="K12" r:id="rId11" xr:uid="{83E0E3A8-8DBB-41C2-A07D-E46E9F04E90B}"/>
+    <hyperlink ref="K13" r:id="rId12" xr:uid="{C75261D1-8074-4479-A01B-A7E7E9177687}"/>
+    <hyperlink ref="K14" r:id="rId13" xr:uid="{ABAB244F-6832-41C3-B584-145326DC26EA}"/>
+    <hyperlink ref="K15" r:id="rId14" xr:uid="{2D7A65A3-4A06-4F98-AD11-AFACE3C6198E}"/>
+    <hyperlink ref="K16" r:id="rId15" xr:uid="{505E0218-2E89-44C5-8F7E-B4933A972984}"/>
+    <hyperlink ref="K17" r:id="rId16" xr:uid="{E74418DE-8B78-4447-9593-586192D39C59}"/>
+    <hyperlink ref="K18" r:id="rId17" xr:uid="{487EFA46-35B6-4A6F-ADD1-8F9089FA752D}"/>
+    <hyperlink ref="K19" r:id="rId18" xr:uid="{9359AC1A-2F35-442F-BB5A-D7387CAFE419}"/>
+    <hyperlink ref="K20" r:id="rId19" xr:uid="{47476116-35F2-4366-8C0E-0E11F7C3F97D}"/>
+    <hyperlink ref="K21" r:id="rId20" xr:uid="{A3A33567-F1D4-45F5-BBB4-E3BC1DE171DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
@@ -3057,16 +3192,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" t="s">
         <v>214</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>215</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>216</v>
-      </c>
-      <c r="D1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4210,19 +4345,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" t="s">
         <v>218</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>219</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>220</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>221</v>
-      </c>
-      <c r="E1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -6973,13 +7108,13 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" t="s">
         <v>212</v>
-      </c>
-      <c r="E1" t="s">
-        <v>213</v>
       </c>
       <c r="F1" t="s">
         <v>20</v>

</xml_diff>